<commit_message>
fix upload rapel manfaat
</commit_message>
<xml_diff>
--- a/public/files/contoh rapel iuran.xlsx
+++ b/public/files/contoh rapel iuran.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bagus Nurcahyo Putra\PERHUTANI\PROJECT DAPEN PERHUTANI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3E629D-04CB-474F-ADCF-066C8D4C9274}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF7AE5B-5514-4966-AE8F-615BC48314E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{0E19FFF5-2BAF-4F21-812C-E6CCD4CE39B2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>NO</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>Ryan</t>
+  </si>
+  <si>
+    <t>tes ubah</t>
+  </si>
+  <si>
+    <t>tes tes ubah</t>
   </si>
 </sst>
 </file>
@@ -194,38 +200,38 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -543,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BB0650C-83BC-43B8-BFD5-EA223C6539B0}">
   <dimension ref="B4:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -553,120 +559,120 @@
     <col min="2" max="2" width="28.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="M7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="N7" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="10">
+      <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="11">
-        <v>1</v>
-      </c>
-      <c r="D10" s="12">
+      <c r="C10" s="4">
+        <v>566</v>
+      </c>
+      <c r="D10" s="5">
         <v>44080</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="4">
         <v>212</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="5">
         <v>43957</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="5">
         <v>43977</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="4">
         <v>10000000</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="4">
         <v>2000000</v>
       </c>
-      <c r="K10" s="13">
+      <c r="K10" s="6">
         <v>11000</v>
       </c>
       <c r="L10" s="1">
@@ -675,36 +681,39 @@
       <c r="M10" s="1">
         <v>4242040200</v>
       </c>
+      <c r="N10" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="10">
+      <c r="B11" s="3">
         <v>2</v>
       </c>
-      <c r="C11" s="11">
-        <v>2</v>
-      </c>
-      <c r="D11" s="12">
+      <c r="C11" s="4">
+        <v>77</v>
+      </c>
+      <c r="D11" s="5">
         <v>40948</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="4">
         <v>211</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="5">
         <v>43957</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="5">
         <v>43977</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="4">
         <v>222222</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="4">
         <v>444444</v>
       </c>
-      <c r="K11" s="13">
+      <c r="K11" s="6">
         <v>113000</v>
       </c>
       <c r="L11" s="1">
@@ -713,36 +722,39 @@
       <c r="M11" s="1">
         <v>2330000</v>
       </c>
+      <c r="N11" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="10">
+      <c r="B12" s="3">
         <v>3</v>
       </c>
-      <c r="C12" s="11">
-        <v>3</v>
-      </c>
-      <c r="D12" s="12">
+      <c r="C12" s="4">
+        <v>23</v>
+      </c>
+      <c r="D12" s="5">
         <v>40948</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="4">
         <v>222</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="5">
         <v>43957</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="5">
         <v>43977</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="4">
         <v>222222</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="4">
         <v>444444</v>
       </c>
-      <c r="K12" s="13">
+      <c r="K12" s="6">
         <v>21000</v>
       </c>
       <c r="L12" s="1">
@@ -751,36 +763,39 @@
       <c r="M12" s="1">
         <v>2392000</v>
       </c>
+      <c r="N12" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="10">
+      <c r="B13" s="3">
         <v>4</v>
       </c>
-      <c r="C13" s="11">
-        <v>4</v>
-      </c>
-      <c r="D13" s="12">
+      <c r="C13" s="4">
+        <v>521</v>
+      </c>
+      <c r="D13" s="5">
         <v>40948</v>
       </c>
-      <c r="E13" s="11">
-        <v>222</v>
-      </c>
-      <c r="F13" s="11" t="s">
+      <c r="E13" s="4">
+        <v>233</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="5">
         <v>43957</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="5">
         <v>43977</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="4">
         <v>222222</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="4">
         <v>444444</v>
       </c>
-      <c r="K13" s="13">
+      <c r="K13" s="6">
         <v>32000</v>
       </c>
       <c r="L13" s="1">
@@ -792,19 +807,19 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
     <mergeCell ref="L7:L9"/>
     <mergeCell ref="M7:M9"/>
     <mergeCell ref="N7:N9"/>
     <mergeCell ref="I7:I9"/>
     <mergeCell ref="J7:J9"/>
     <mergeCell ref="K7:K9"/>
+    <mergeCell ref="H7:H9"/>
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="G7:G9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="H7:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>